<commit_message>
Matches: Acomode el nombre de ON en algunas partidas
proyecto: Terminé la caja de informacion extra para los jugadores y comence la de los campeones
</commit_message>
<xml_diff>
--- a/matches.xlsx
+++ b/matches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\iCentro\Desktop\Escritorio\Facu\Analisis exploratorio de datos (Shiny)\Proyecto-WORLDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542B707D-EA6D-4BDA-B054-BB8EC536EBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C880734B-E327-48CD-A15B-74A700DA05C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6C6FBEDB-E842-4995-A78D-B58436CB68C0}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="8310" xr2:uid="{6C6FBEDB-E842-4995-A78D-B58436CB68C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="318">
   <si>
     <t>Date</t>
   </si>
@@ -589,9 +589,6 @@
   </si>
   <si>
     <t>CoreJJ</t>
-  </si>
-  <si>
-    <t>0N</t>
   </si>
   <si>
     <t>BTC</t>
@@ -1368,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624D0EFB-10A1-43D7-87F4-77EB0B831DD5}">
   <dimension ref="A1:AV80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="W73" sqref="W73"/>
+    <sheetView tabSelected="1" topLeftCell="K58" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AF76" sqref="AF76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1394,94 +1391,94 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>4</v>
@@ -1528,7 +1525,7 @@
         <v>45249.447222222225</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
@@ -1609,7 +1606,7 @@
         <v>121</v>
       </c>
       <c r="AC2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AD2" t="s">
         <v>122</v>
@@ -1630,7 +1627,7 @@
         <v>130</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AK2" s="3">
         <v>41229</v>
@@ -1674,7 +1671,7 @@
         <v>45249.410416666666</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -1755,7 +1752,7 @@
         <v>121</v>
       </c>
       <c r="AC3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AD3" t="s">
         <v>122</v>
@@ -1776,7 +1773,7 @@
         <v>130</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK3" s="3">
         <v>45122</v>
@@ -1820,7 +1817,7 @@
         <v>45249.372916666667</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
@@ -1901,7 +1898,7 @@
         <v>121</v>
       </c>
       <c r="AC4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AD4" t="s">
         <v>122</v>
@@ -1922,7 +1919,7 @@
         <v>130</v>
       </c>
       <c r="AJ4" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AK4" s="3">
         <v>49024</v>
@@ -1966,7 +1963,7 @@
         <v>45242.450694444444</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>19</v>
@@ -2044,7 +2041,7 @@
         <v>123</v>
       </c>
       <c r="AB5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AC5" t="s">
         <v>124</v>
@@ -2068,7 +2065,7 @@
         <v>130</v>
       </c>
       <c r="AJ5" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AK5" s="3">
         <v>51388</v>
@@ -2112,7 +2109,7 @@
         <v>45242.415972222225</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>18</v>
@@ -2148,7 +2145,7 @@
         <v>61</v>
       </c>
       <c r="N6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O6" t="s">
         <v>40</v>
@@ -2205,7 +2202,7 @@
         <v>123</v>
       </c>
       <c r="AG6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AH6" t="s">
         <v>124</v>
@@ -2214,7 +2211,7 @@
         <v>125</v>
       </c>
       <c r="AJ6" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AK6" s="3">
         <v>55267</v>
@@ -2258,7 +2255,7 @@
         <v>45242.375694444447</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
@@ -2336,7 +2333,7 @@
         <v>123</v>
       </c>
       <c r="AB7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AC7" t="s">
         <v>124</v>
@@ -2404,7 +2401,7 @@
         <v>45242.345138888886</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>18</v>
@@ -2497,7 +2494,7 @@
         <v>123</v>
       </c>
       <c r="AG8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AH8" t="s">
         <v>124</v>
@@ -2506,7 +2503,7 @@
         <v>125</v>
       </c>
       <c r="AJ8" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AK8" s="3">
         <v>48178</v>
@@ -2550,7 +2547,7 @@
         <v>45241.484027777777</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>17</v>
@@ -2631,13 +2628,13 @@
         <v>121</v>
       </c>
       <c r="AC9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AD9" t="s">
         <v>122</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF9" t="s">
         <v>131</v>
@@ -2652,7 +2649,7 @@
         <v>134</v>
       </c>
       <c r="AJ9" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AK9" s="3">
         <v>64526</v>
@@ -2696,7 +2693,7 @@
         <v>45241.451388888891</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>21</v>
@@ -2768,7 +2765,7 @@
         <v>109</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA10" t="s">
         <v>131</v>
@@ -2792,13 +2789,13 @@
         <v>121</v>
       </c>
       <c r="AH10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI10" t="s">
         <v>122</v>
       </c>
       <c r="AJ10" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AK10" s="3">
         <v>56853</v>
@@ -2842,7 +2839,7 @@
         <v>45241.417361111111</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>17</v>
@@ -2923,13 +2920,13 @@
         <v>121</v>
       </c>
       <c r="AC11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AD11" t="s">
         <v>122</v>
       </c>
       <c r="AE11" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF11" t="s">
         <v>131</v>
@@ -2944,7 +2941,7 @@
         <v>134</v>
       </c>
       <c r="AJ11" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AK11" s="3">
         <v>52694</v>
@@ -2988,7 +2985,7 @@
         <v>45241.379861111112</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>21</v>
@@ -3060,7 +3057,7 @@
         <v>96</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA12" t="s">
         <v>131</v>
@@ -3084,13 +3081,13 @@
         <v>121</v>
       </c>
       <c r="AH12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI12" t="s">
         <v>122</v>
       </c>
       <c r="AJ12" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AK12" s="3">
         <v>73260</v>
@@ -3134,7 +3131,7 @@
         <v>45241.345138888886</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>17</v>
@@ -3215,13 +3212,13 @@
         <v>121</v>
       </c>
       <c r="AC13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AD13" t="s">
         <v>122</v>
       </c>
       <c r="AE13" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF13" t="s">
         <v>131</v>
@@ -3236,7 +3233,7 @@
         <v>134</v>
       </c>
       <c r="AJ13" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AK13" s="3">
         <v>59187</v>
@@ -3280,7 +3277,7 @@
         <v>45235.409722222219</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>22</v>
@@ -3355,7 +3352,7 @@
         <v>135</v>
       </c>
       <c r="AA14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AB14" t="s">
         <v>136</v>
@@ -3382,7 +3379,7 @@
         <v>130</v>
       </c>
       <c r="AJ14" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AK14" s="3">
         <v>40096</v>
@@ -3426,7 +3423,7 @@
         <v>45235.373611111114</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>22</v>
@@ -3501,7 +3498,7 @@
         <v>135</v>
       </c>
       <c r="AA15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AB15" t="s">
         <v>136</v>
@@ -3528,7 +3525,7 @@
         <v>130</v>
       </c>
       <c r="AJ15" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AK15" s="3">
         <v>49147</v>
@@ -3572,7 +3569,7 @@
         <v>45235.341666666667</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>22</v>
@@ -3647,7 +3644,7 @@
         <v>135</v>
       </c>
       <c r="AA16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AB16" t="s">
         <v>136</v>
@@ -3674,7 +3671,7 @@
         <v>130</v>
       </c>
       <c r="AJ16" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK16" s="3">
         <v>41532</v>
@@ -3718,7 +3715,7 @@
         <v>45234.44027777778</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>23</v>
@@ -3811,7 +3808,7 @@
         <v>123</v>
       </c>
       <c r="AG17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AH17" t="s">
         <v>124</v>
@@ -3820,7 +3817,7 @@
         <v>125</v>
       </c>
       <c r="AJ17" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AK17" s="3">
         <v>60151</v>
@@ -3864,7 +3861,7 @@
         <v>45234.408333333333</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>23</v>
@@ -3957,7 +3954,7 @@
         <v>123</v>
       </c>
       <c r="AG18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AH18" t="s">
         <v>124</v>
@@ -3966,7 +3963,7 @@
         <v>125</v>
       </c>
       <c r="AJ18" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AK18" s="3">
         <v>44433</v>
@@ -4010,7 +4007,7 @@
         <v>45234.376388888886</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>19</v>
@@ -4088,7 +4085,7 @@
         <v>123</v>
       </c>
       <c r="AB19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AC19" t="s">
         <v>124</v>
@@ -4156,7 +4153,7 @@
         <v>45234.342361111114</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>19</v>
@@ -4234,7 +4231,7 @@
         <v>123</v>
       </c>
       <c r="AB20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AC20" t="s">
         <v>124</v>
@@ -4258,7 +4255,7 @@
         <v>143</v>
       </c>
       <c r="AJ20" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AK20" s="3">
         <v>48069</v>
@@ -4302,7 +4299,7 @@
         <v>45233.495833333334</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>21</v>
@@ -4374,7 +4371,7 @@
         <v>51</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA21" t="s">
         <v>131</v>
@@ -4389,7 +4386,7 @@
         <v>134</v>
       </c>
       <c r="AE21" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AF21" t="s">
         <v>144</v>
@@ -4404,7 +4401,7 @@
         <v>147</v>
       </c>
       <c r="AJ21" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AK21" s="3">
         <v>63411</v>
@@ -4448,7 +4445,7 @@
         <v>45233.457638888889</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>21</v>
@@ -4520,7 +4517,7 @@
         <v>51</v>
       </c>
       <c r="Z22" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA22" t="s">
         <v>131</v>
@@ -4535,7 +4532,7 @@
         <v>134</v>
       </c>
       <c r="AE22" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AF22" t="s">
         <v>144</v>
@@ -4550,7 +4547,7 @@
         <v>147</v>
       </c>
       <c r="AJ22" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AK22" s="3">
         <v>60190</v>
@@ -4594,7 +4591,7 @@
         <v>45233.411805555559</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>25</v>
@@ -4666,7 +4663,7 @@
         <v>82</v>
       </c>
       <c r="Z23" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA23" t="s">
         <v>144</v>
@@ -4681,7 +4678,7 @@
         <v>147</v>
       </c>
       <c r="AE23" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF23" t="s">
         <v>131</v>
@@ -4696,7 +4693,7 @@
         <v>134</v>
       </c>
       <c r="AJ23" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AK23" s="3">
         <v>90253</v>
@@ -4740,7 +4737,7 @@
         <v>45233.379166666666</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>21</v>
@@ -4812,7 +4809,7 @@
         <v>67</v>
       </c>
       <c r="Z24" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA24" t="s">
         <v>131</v>
@@ -4827,7 +4824,7 @@
         <v>134</v>
       </c>
       <c r="AE24" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AF24" t="s">
         <v>144</v>
@@ -4842,7 +4839,7 @@
         <v>147</v>
       </c>
       <c r="AJ24" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AK24" s="3">
         <v>58761</v>
@@ -4881,12 +4878,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:48" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45233.341666666667</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>25</v>
@@ -4958,7 +4955,7 @@
         <v>52</v>
       </c>
       <c r="Z25" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA25" t="s">
         <v>144</v>
@@ -4973,7 +4970,7 @@
         <v>147</v>
       </c>
       <c r="AE25" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF25" t="s">
         <v>131</v>
@@ -4988,7 +4985,7 @@
         <v>134</v>
       </c>
       <c r="AJ25" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AK25" s="3">
         <v>48578</v>
@@ -5032,7 +5029,7 @@
         <v>45232.420138888891</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>26</v>
@@ -5128,13 +5125,13 @@
         <v>121</v>
       </c>
       <c r="AH26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI26" t="s">
         <v>122</v>
       </c>
       <c r="AJ26" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AK26" s="3">
         <v>40879</v>
@@ -5178,7 +5175,7 @@
         <v>45232.383333333331</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>26</v>
@@ -5274,13 +5271,13 @@
         <v>121</v>
       </c>
       <c r="AH27" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI27" t="s">
         <v>122</v>
       </c>
       <c r="AJ27" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AK27" s="3">
         <v>53863</v>
@@ -5324,7 +5321,7 @@
         <v>45232.342361111114</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>26</v>
@@ -5420,13 +5417,13 @@
         <v>121</v>
       </c>
       <c r="AH28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI28" t="s">
         <v>122</v>
       </c>
       <c r="AJ28" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AK28" s="3">
         <v>65145</v>
@@ -5470,7 +5467,7 @@
         <v>45228.45</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>21</v>
@@ -5542,7 +5539,7 @@
         <v>40</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA29" t="s">
         <v>131</v>
@@ -5572,7 +5569,7 @@
         <v>157</v>
       </c>
       <c r="AJ29" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AK29" s="3">
         <v>57612</v>
@@ -5616,7 +5613,7 @@
         <v>45228.405555555553</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>27</v>
@@ -5703,7 +5700,7 @@
         <v>157</v>
       </c>
       <c r="AE30" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF30" t="s">
         <v>131</v>
@@ -5718,7 +5715,7 @@
         <v>134</v>
       </c>
       <c r="AJ30" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AK30" s="3">
         <v>83973</v>
@@ -5762,7 +5759,7 @@
         <v>45228.365277777775</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>27</v>
@@ -5849,7 +5846,7 @@
         <v>157</v>
       </c>
       <c r="AE31" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF31" t="s">
         <v>131</v>
@@ -5864,7 +5861,7 @@
         <v>134</v>
       </c>
       <c r="AJ31" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AK31" s="3">
         <v>54139</v>
@@ -5908,7 +5905,7 @@
         <v>45228.331944444442</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>28</v>
@@ -5989,7 +5986,7 @@
         <v>160</v>
       </c>
       <c r="AC32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AD32" t="s">
         <v>161</v>
@@ -6004,13 +6001,13 @@
         <v>121</v>
       </c>
       <c r="AH32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI32" t="s">
         <v>122</v>
       </c>
       <c r="AJ32" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AK32" s="3">
         <v>40109</v>
@@ -6054,7 +6051,7 @@
         <v>45228.29583333333</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>17</v>
@@ -6135,7 +6132,7 @@
         <v>121</v>
       </c>
       <c r="AC33" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AD33" t="s">
         <v>122</v>
@@ -6150,13 +6147,13 @@
         <v>160</v>
       </c>
       <c r="AH33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AI33" t="s">
         <v>161</v>
       </c>
       <c r="AJ33" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AK33" s="3">
         <v>63375</v>
@@ -6200,7 +6197,7 @@
         <v>45228.259027777778</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>28</v>
@@ -6281,7 +6278,7 @@
         <v>160</v>
       </c>
       <c r="AC34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AD34" t="s">
         <v>161</v>
@@ -6296,13 +6293,13 @@
         <v>121</v>
       </c>
       <c r="AH34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI34" t="s">
         <v>122</v>
       </c>
       <c r="AJ34" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AK34" s="3">
         <v>54145</v>
@@ -6346,7 +6343,7 @@
         <v>45228.211111111108</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>29</v>
@@ -6448,7 +6445,7 @@
         <v>143</v>
       </c>
       <c r="AJ35" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AK35" s="3">
         <v>77706</v>
@@ -6492,7 +6489,7 @@
         <v>45228.173611111109</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>23</v>
@@ -6594,7 +6591,7 @@
         <v>166</v>
       </c>
       <c r="AJ36" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AK36" s="3">
         <v>70428</v>
@@ -6638,7 +6635,7 @@
         <v>45227.40625</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>21</v>
@@ -6710,7 +6707,7 @@
         <v>47</v>
       </c>
       <c r="Z37" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA37" t="s">
         <v>131</v>
@@ -6740,7 +6737,7 @@
         <v>130</v>
       </c>
       <c r="AJ37" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AK37" s="3">
         <v>49962</v>
@@ -6784,7 +6781,7 @@
         <v>45227.372916666667</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>18</v>
@@ -6871,7 +6868,7 @@
         <v>130</v>
       </c>
       <c r="AE38" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF38" t="s">
         <v>131</v>
@@ -6886,7 +6883,7 @@
         <v>134</v>
       </c>
       <c r="AJ38" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AK38" s="3">
         <v>57171</v>
@@ -6930,7 +6927,7 @@
         <v>45227.336805555555</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>27</v>
@@ -7032,7 +7029,7 @@
         <v>152</v>
       </c>
       <c r="AJ39" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AK39" s="3">
         <v>46160</v>
@@ -7076,7 +7073,7 @@
         <v>45227.3</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>26</v>
@@ -7178,7 +7175,7 @@
         <v>157</v>
       </c>
       <c r="AJ40" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AK40" s="3">
         <v>62010</v>
@@ -7222,7 +7219,7 @@
         <v>45226.444444444445</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>22</v>
@@ -7297,7 +7294,7 @@
         <v>135</v>
       </c>
       <c r="AA41" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AB41" t="s">
         <v>136</v>
@@ -7324,7 +7321,7 @@
         <v>143</v>
       </c>
       <c r="AJ41" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AK41" s="3">
         <v>49884</v>
@@ -7368,7 +7365,7 @@
         <v>45226.407638888886</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>23</v>
@@ -7458,7 +7455,7 @@
         <v>135</v>
       </c>
       <c r="AF42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AG42" t="s">
         <v>136</v>
@@ -7470,7 +7467,7 @@
         <v>138</v>
       </c>
       <c r="AJ42" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AK42" s="3">
         <v>65080</v>
@@ -7514,7 +7511,7 @@
         <v>45226.368750000001</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>23</v>
@@ -7604,7 +7601,7 @@
         <v>135</v>
       </c>
       <c r="AF43" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AG43" t="s">
         <v>136</v>
@@ -7616,7 +7613,7 @@
         <v>138</v>
       </c>
       <c r="AJ43" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AK43" s="3">
         <v>58245</v>
@@ -7660,7 +7657,7 @@
         <v>45226.334027777775</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>30</v>
@@ -7762,7 +7759,7 @@
         <v>166</v>
       </c>
       <c r="AJ44" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AK44" s="3">
         <v>39854</v>
@@ -7806,7 +7803,7 @@
         <v>45226.300694444442</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>29</v>
@@ -7908,7 +7905,7 @@
         <v>171</v>
       </c>
       <c r="AJ45" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AK45" s="3">
         <v>52392</v>
@@ -7952,7 +7949,7 @@
         <v>45225.454861111109</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>31</v>
@@ -7991,7 +7988,7 @@
         <v>73</v>
       </c>
       <c r="O46" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P46" s="3" t="s">
         <v>53</v>
@@ -8048,13 +8045,13 @@
         <v>121</v>
       </c>
       <c r="AH46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI46" t="s">
         <v>122</v>
       </c>
       <c r="AJ46" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AK46" s="3">
         <v>45439</v>
@@ -8098,7 +8095,7 @@
         <v>45225.415277777778</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>31</v>
@@ -8194,13 +8191,13 @@
         <v>121</v>
       </c>
       <c r="AH47" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI47" t="s">
         <v>122</v>
       </c>
       <c r="AJ47" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AK47" s="3">
         <v>54127</v>
@@ -8244,7 +8241,7 @@
         <v>45225.374305555553</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>32</v>
@@ -8325,7 +8322,7 @@
         <v>179</v>
       </c>
       <c r="AC48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AD48" t="s">
         <v>180</v>
@@ -8340,13 +8337,13 @@
         <v>160</v>
       </c>
       <c r="AH48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AI48" t="s">
         <v>161</v>
       </c>
       <c r="AJ48" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AK48" s="3">
         <v>58897</v>
@@ -8390,7 +8387,7 @@
         <v>45225.341666666667</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>28</v>
@@ -8471,7 +8468,7 @@
         <v>160</v>
       </c>
       <c r="AC49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AD49" t="s">
         <v>161</v>
@@ -8486,13 +8483,13 @@
         <v>179</v>
       </c>
       <c r="AH49" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AI49" t="s">
         <v>180</v>
       </c>
       <c r="AJ49" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AK49" s="3">
         <v>59092</v>
@@ -8536,7 +8533,7 @@
         <v>45225.299305555556</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>32</v>
@@ -8617,7 +8614,7 @@
         <v>179</v>
       </c>
       <c r="AC50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AD50" t="s">
         <v>180</v>
@@ -8632,13 +8629,13 @@
         <v>160</v>
       </c>
       <c r="AH50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AI50" t="s">
         <v>161</v>
       </c>
       <c r="AJ50" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AK50" s="3">
         <v>82088</v>
@@ -8677,12 +8674,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:48" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45222.441666666666</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>33</v>
@@ -8706,13 +8703,13 @@
         <v>94</v>
       </c>
       <c r="J51" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K51" s="3" t="s">
         <v>42</v>
       </c>
       <c r="L51" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M51" t="s">
         <v>48</v>
@@ -8754,7 +8751,7 @@
         <v>80</v>
       </c>
       <c r="Z51" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AA51" t="s">
         <v>181</v>
@@ -8784,7 +8781,7 @@
         <v>166</v>
       </c>
       <c r="AJ51" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AK51" s="3">
         <v>40238</v>
@@ -8823,12 +8820,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:48" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45222.410416666666</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>29</v>
@@ -8843,7 +8840,7 @@
         <v>42</v>
       </c>
       <c r="G52" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H52" t="s">
         <v>48</v>
@@ -8852,7 +8849,7 @@
         <v>106</v>
       </c>
       <c r="J52" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K52" s="3" t="s">
         <v>44</v>
@@ -8915,7 +8912,7 @@
         <v>166</v>
       </c>
       <c r="AE52" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AF52" t="s">
         <v>181</v>
@@ -8930,7 +8927,7 @@
         <v>184</v>
       </c>
       <c r="AJ52" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AK52" s="3">
         <v>52046</v>
@@ -8974,7 +8971,7 @@
         <v>45222.365972222222</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>30</v>
@@ -9067,16 +9064,16 @@
         <v>186</v>
       </c>
       <c r="AG53" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AH53" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AI53" t="s">
         <v>187</v>
       </c>
       <c r="AJ53" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AK53" s="3">
         <v>69267</v>
@@ -9120,7 +9117,7 @@
         <v>45222.334027777775</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>34</v>
@@ -9198,10 +9195,10 @@
         <v>186</v>
       </c>
       <c r="AB54" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AC54" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AD54" t="s">
         <v>187</v>
@@ -9222,7 +9219,7 @@
         <v>171</v>
       </c>
       <c r="AJ54" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AK54" s="3">
         <v>49326</v>
@@ -9266,7 +9263,7 @@
         <v>45222.3</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>34</v>
@@ -9344,10 +9341,10 @@
         <v>186</v>
       </c>
       <c r="AB55" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AC55" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AD55" t="s">
         <v>187</v>
@@ -9368,7 +9365,7 @@
         <v>171</v>
       </c>
       <c r="AJ55" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AK55" s="3">
         <v>45274</v>
@@ -9412,7 +9409,7 @@
         <v>45221.42083333333</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>23</v>
@@ -9508,13 +9505,13 @@
         <v>121</v>
       </c>
       <c r="AH56" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI56" t="s">
         <v>122</v>
       </c>
       <c r="AJ56" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AK56" s="3">
         <v>76480</v>
@@ -9558,7 +9555,7 @@
         <v>45221.381249999999</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>21</v>
@@ -9630,7 +9627,7 @@
         <v>80</v>
       </c>
       <c r="Z57" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA57" t="s">
         <v>131</v>
@@ -9654,13 +9651,13 @@
         <v>160</v>
       </c>
       <c r="AH57" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AI57" t="s">
         <v>161</v>
       </c>
       <c r="AJ57" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AK57" s="3">
         <v>64084</v>
@@ -9704,7 +9701,7 @@
         <v>45221.331944444442</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>26</v>
@@ -9806,7 +9803,7 @@
         <v>176</v>
       </c>
       <c r="AJ58" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AK58" s="3">
         <v>79248</v>
@@ -9850,7 +9847,7 @@
         <v>45221.299305555556</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>18</v>
@@ -9946,13 +9943,13 @@
         <v>179</v>
       </c>
       <c r="AH59" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AI59" t="s">
         <v>180</v>
       </c>
       <c r="AJ59" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AK59" s="3">
         <v>48782</v>
@@ -9991,12 +9988,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:48" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>45220.436111111114</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>27</v>
@@ -10083,7 +10080,7 @@
         <v>157</v>
       </c>
       <c r="AE60" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AF60" t="s">
         <v>144</v>
@@ -10098,7 +10095,7 @@
         <v>147</v>
       </c>
       <c r="AJ60" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AK60" s="3">
         <v>52798</v>
@@ -10137,12 +10134,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:48" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>45220.401388888888</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>27</v>
@@ -10229,7 +10226,7 @@
         <v>157</v>
       </c>
       <c r="AE61" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AF61" t="s">
         <v>144</v>
@@ -10244,7 +10241,7 @@
         <v>147</v>
       </c>
       <c r="AJ61" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AK61" s="3">
         <v>53369</v>
@@ -10288,7 +10285,7 @@
         <v>45220.365972222222</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>19</v>
@@ -10366,7 +10363,7 @@
         <v>123</v>
       </c>
       <c r="AB62" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AC62" t="s">
         <v>124</v>
@@ -10378,7 +10375,7 @@
         <v>135</v>
       </c>
       <c r="AF62" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AG62" t="s">
         <v>136</v>
@@ -10390,7 +10387,7 @@
         <v>138</v>
       </c>
       <c r="AJ62" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AK62" s="3">
         <v>52486</v>
@@ -10434,7 +10431,7 @@
         <v>45220.331944444442</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>22</v>
@@ -10509,7 +10506,7 @@
         <v>135</v>
       </c>
       <c r="AA63" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AB63" t="s">
         <v>136</v>
@@ -10527,7 +10524,7 @@
         <v>123</v>
       </c>
       <c r="AG63" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AH63" t="s">
         <v>124</v>
@@ -10536,7 +10533,7 @@
         <v>125</v>
       </c>
       <c r="AJ63" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AK63" s="3">
         <v>57330</v>
@@ -10580,7 +10577,7 @@
         <v>45220.299305555556</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>19</v>
@@ -10658,7 +10655,7 @@
         <v>123</v>
       </c>
       <c r="AB64" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AC64" t="s">
         <v>124</v>
@@ -10670,7 +10667,7 @@
         <v>135</v>
       </c>
       <c r="AF64" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AG64" t="s">
         <v>136</v>
@@ -10682,7 +10679,7 @@
         <v>138</v>
       </c>
       <c r="AJ64" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AK64" s="3">
         <v>55280</v>
@@ -10726,7 +10723,7 @@
         <v>45219.508333333331</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>29</v>
@@ -10828,7 +10825,7 @@
         <v>143</v>
       </c>
       <c r="AJ65" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AK65" s="3">
         <v>51313</v>
@@ -10872,7 +10869,7 @@
         <v>45219.474305555559</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>19</v>
@@ -10950,7 +10947,7 @@
         <v>123</v>
       </c>
       <c r="AB66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AC66" t="s">
         <v>124</v>
@@ -10959,7 +10956,7 @@
         <v>125</v>
       </c>
       <c r="AE66" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF66" t="s">
         <v>131</v>
@@ -10974,7 +10971,7 @@
         <v>134</v>
       </c>
       <c r="AJ66" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AK66" s="3">
         <v>52171</v>
@@ -11018,7 +11015,7 @@
         <v>45219.427777777775</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>27</v>
@@ -11114,13 +11111,13 @@
         <v>121</v>
       </c>
       <c r="AH67" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI67" t="s">
         <v>122</v>
       </c>
       <c r="AJ67" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AK67" s="3">
         <v>75520</v>
@@ -11164,7 +11161,7 @@
         <v>45219.38958333333</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>25</v>
@@ -11236,7 +11233,7 @@
         <v>80</v>
       </c>
       <c r="Z68" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA68" t="s">
         <v>144</v>
@@ -11266,7 +11263,7 @@
         <v>130</v>
       </c>
       <c r="AJ68" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AK68" s="3">
         <v>58370</v>
@@ -11310,7 +11307,7 @@
         <v>45219.353472222225</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>28</v>
@@ -11391,7 +11388,7 @@
         <v>160</v>
       </c>
       <c r="AC69" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AD69" t="s">
         <v>161</v>
@@ -11412,7 +11409,7 @@
         <v>171</v>
       </c>
       <c r="AJ69" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AK69" s="3">
         <v>49855</v>
@@ -11456,7 +11453,7 @@
         <v>45219.314583333333</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>31</v>
@@ -11471,7 +11468,7 @@
         <v>42</v>
       </c>
       <c r="G70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H70" t="s">
         <v>48</v>
@@ -11543,7 +11540,7 @@
         <v>176</v>
       </c>
       <c r="AE70" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AF70" t="s">
         <v>181</v>
@@ -11558,7 +11555,7 @@
         <v>184</v>
       </c>
       <c r="AJ70" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AK70" s="3">
         <v>65500</v>
@@ -11602,7 +11599,7 @@
         <v>45219.285416666666</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>32</v>
@@ -11683,7 +11680,7 @@
         <v>179</v>
       </c>
       <c r="AC71" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AD71" t="s">
         <v>180</v>
@@ -11692,7 +11689,7 @@
         <v>135</v>
       </c>
       <c r="AF71" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AG71" t="s">
         <v>136</v>
@@ -11704,7 +11701,7 @@
         <v>138</v>
       </c>
       <c r="AJ71" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AK71" s="3">
         <v>55531</v>
@@ -11748,7 +11745,7 @@
         <v>45219.21597222222</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>26</v>
@@ -11841,16 +11838,16 @@
         <v>186</v>
       </c>
       <c r="AG72" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AH72" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AI72" t="s">
         <v>187</v>
       </c>
       <c r="AJ72" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AK72" s="3">
         <v>60491</v>
@@ -11894,7 +11891,7 @@
         <v>45218.522916666669</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>21</v>
@@ -11966,7 +11963,7 @@
         <v>70</v>
       </c>
       <c r="Z73" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA73" t="s">
         <v>131</v>
@@ -11978,7 +11975,7 @@
         <v>133</v>
       </c>
       <c r="AD73" t="s">
-        <v>188</v>
+        <v>134</v>
       </c>
       <c r="AE73" s="3" t="s">
         <v>139</v>
@@ -11996,7 +11993,7 @@
         <v>143</v>
       </c>
       <c r="AJ73" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AK73" s="3">
         <v>85814</v>
@@ -12040,7 +12037,7 @@
         <v>45218.48333333333</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>22</v>
@@ -12115,7 +12112,7 @@
         <v>135</v>
       </c>
       <c r="AA74" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AB74" t="s">
         <v>136</v>
@@ -12136,13 +12133,13 @@
         <v>160</v>
       </c>
       <c r="AH74" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AI74" t="s">
         <v>161</v>
       </c>
       <c r="AJ74" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AK74" s="3">
         <v>60844</v>
@@ -12186,7 +12183,7 @@
         <v>45218.444444444445</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>17</v>
@@ -12267,7 +12264,7 @@
         <v>121</v>
       </c>
       <c r="AC75" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AD75" t="s">
         <v>122</v>
@@ -12288,7 +12285,7 @@
         <v>152</v>
       </c>
       <c r="AJ75" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AK75" s="3">
         <v>61041</v>
@@ -12332,7 +12329,7 @@
         <v>45218.392361111109</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>27</v>
@@ -12371,7 +12368,7 @@
         <v>57</v>
       </c>
       <c r="O76" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P76" s="3" t="s">
         <v>68</v>
@@ -12434,7 +12431,7 @@
         <v>166</v>
       </c>
       <c r="AJ76" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AK76" s="3">
         <v>80837</v>
@@ -12478,7 +12475,7 @@
         <v>45218.354166666664</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>33</v>
@@ -12505,7 +12502,7 @@
         <v>68</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L77" t="s">
         <v>48</v>
@@ -12550,7 +12547,7 @@
         <v>80</v>
       </c>
       <c r="Z77" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AA77" t="s">
         <v>181</v>
@@ -12571,7 +12568,7 @@
         <v>123</v>
       </c>
       <c r="AG77" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AH77" t="s">
         <v>124</v>
@@ -12580,7 +12577,7 @@
         <v>125</v>
       </c>
       <c r="AJ77" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AK77" s="3">
         <v>46972</v>
@@ -12624,7 +12621,7 @@
         <v>45218.30972222222</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>25</v>
@@ -12696,7 +12693,7 @@
         <v>118</v>
       </c>
       <c r="Z78" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA78" t="s">
         <v>144</v>
@@ -12726,7 +12723,7 @@
         <v>171</v>
       </c>
       <c r="AJ78" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AK78" s="3">
         <v>50430</v>
@@ -12770,7 +12767,7 @@
         <v>45218.268750000003</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>32</v>
@@ -12851,7 +12848,7 @@
         <v>179</v>
       </c>
       <c r="AC79" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AD79" t="s">
         <v>180</v>
@@ -12916,7 +12913,7 @@
         <v>45218.219444444447</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>18</v>
@@ -13009,16 +13006,16 @@
         <v>186</v>
       </c>
       <c r="AG80" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AH80" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AI80" t="s">
         <v>187</v>
       </c>
       <c r="AJ80" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AK80" s="3">
         <v>67196</v>

</xml_diff>